<commit_message>
add polymorphic relation in party and contact table
</commit_message>
<xml_diff>
--- a/doc/Requirement.xlsx
+++ b/doc/Requirement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Electron\react-electron\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FE694DF-0B51-4FB8-A9E9-3B7D68E86309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7296A2F5-2F91-4550-9ED1-582360A41EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8D0D73FC-725E-45A3-82B2-FDC9ACA54A8D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D0D73FC-725E-45A3-82B2-FDC9ACA54A8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Parties" sheetId="1" r:id="rId1"/>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FB0400-AF7C-4E4E-A7FC-9DE592D09DC3}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C188D3-4ADB-4549-91A0-F3682123CFCA}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>